<commit_message>
Diego Saavedra -- Se realiza ajustes a Reporte de Amonestados para que las fechas se generen de manera Vertical
</commit_message>
<xml_diff>
--- a/JCA_Futbol_Admin/Utiles/ReporteAmonestados.xlsx
+++ b/JCA_Futbol_Admin/Utiles/ReporteAmonestados.xlsx
@@ -21,27 +21,43 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Equipo</t>
+    <t>No</t>
   </si>
   <si>
-    <t>Jugador</t>
+    <t>EQUIPO</t>
   </si>
   <si>
-    <t>CAMPEONATO</t>
+    <t>JUGADOR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -51,8 +67,26 @@
     <fill>
       <patternFill patternType="none"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -60,12 +94,89 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -370,30 +481,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.54296875" customWidth="1"/>
+    <col min="1" max="1" width="16.1796875" customWidth="1"/>
+    <col min="2" max="2" width="29.08984375" customWidth="1"/>
+    <col min="3" max="3" width="52.7265625" customWidth="1"/>
+    <col min="4" max="4" width="12.7265625" customWidth="1"/>
+    <col min="5" max="5" width="12.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" ht="23.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+    </row>
+    <row r="2" spans="1:5" ht="21.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:5" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>